<commit_message>
Integrazione documentazione ANSC V1.43.0
</commit_message>
<xml_diff>
--- a/docs/Mapping_casi_uso/3_dec_use_case.xlsx
+++ b/docs/Mapping_casi_uso/3_dec_use_case.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="682">
   <si>
     <t>ID USECASE</t>
   </si>
@@ -930,6 +930,12 @@
   </si>
   <si>
     <t>Rico_015</t>
+  </si>
+  <si>
+    <t>12422300</t>
+  </si>
+  <si>
+    <t>Rico_021</t>
   </si>
   <si>
     <t>12999999</t>
@@ -2110,7 +2116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C340"/>
+  <dimension ref="A1:C341"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4840,6 +4846,14 @@
         <v>679</v>
       </c>
     </row>
+    <row r="341">
+      <c r="A341" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>